<commit_message>
Modified month12.r, added volumes and resid csv files.
Modified Month 36 to check for missing subjects.

Revised Month 48 to match previous R scripts.
</commit_message>
<xml_diff>
--- a/DxMonth48.xlsx
+++ b/DxMonth48.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salahmekhalalati/Documents/R_projects/Listingvols/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salah\Documents\R _projects\ADNI_Hippocampus_Dataframes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1404EF1-9F92-274F-84B0-C88940081650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CE18F8-23C3-421C-82BE-9125311C06BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2740" windowWidth="26440" windowHeight="15260" xr2:uid="{F6415A73-CB27-E342-A519-1BFB50FADC43}"/>
+    <workbookView xWindow="390" yWindow="360" windowWidth="18195" windowHeight="11160" xr2:uid="{F6415A73-CB27-E342-A519-1BFB50FADC43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>RID</t>
   </si>
   <si>
-    <t>PTID</t>
-  </si>
-  <si>
     <t>SITEID</t>
   </si>
   <si>
@@ -512,6 +509,9 @@
   </si>
   <si>
     <t>136_S_0186</t>
+  </si>
+  <si>
+    <t>subject</t>
   </si>
 </sst>
 </file>
@@ -869,12 +869,12 @@
   <dimension ref="A1:BB102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -885,162 +885,162 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>54</v>
       </c>
       <c r="B2">
         <v>7434</v>
@@ -1049,16 +1049,16 @@
         <v>295</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2">
         <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2" s="1">
         <v>40312</v>
@@ -1178,9 +1178,9 @@
         <v>40312</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>7418</v>
@@ -1189,16 +1189,16 @@
         <v>413</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3">
         <v>101</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3" s="1">
         <v>40304</v>
@@ -1318,9 +1318,9 @@
         <v>40304</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>7296</v>
@@ -1329,16 +1329,16 @@
         <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H4" s="1">
         <v>40235</v>
@@ -1458,9 +1458,9 @@
         <v>40235</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>7202</v>
@@ -1469,16 +1469,16 @@
         <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="1">
         <v>40212</v>
@@ -1598,9 +1598,9 @@
         <v>40212</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6">
         <v>7206</v>
@@ -1609,16 +1609,16 @@
         <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H6" s="1">
         <v>40213</v>
@@ -1738,9 +1738,9 @@
         <v>40213</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>7298</v>
@@ -1749,16 +1749,16 @@
         <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" s="1">
         <v>40235</v>
@@ -1878,9 +1878,9 @@
         <v>40235</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>7492</v>
@@ -1889,16 +1889,16 @@
         <v>249</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="1">
         <v>40358</v>
@@ -2018,9 +2018,9 @@
         <v>40358</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>7490</v>
@@ -2029,16 +2029,16 @@
         <v>344</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" s="1">
         <v>40358</v>
@@ -2158,9 +2158,9 @@
         <v>40358</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10">
         <v>7512</v>
@@ -2169,16 +2169,16 @@
         <v>419</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10">
         <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" s="1">
         <v>40380</v>
@@ -2298,9 +2298,9 @@
         <v>40380</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11">
         <v>7154</v>
@@ -2309,16 +2309,16 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11">
         <v>107</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" s="1">
         <v>40189</v>
@@ -2438,9 +2438,9 @@
         <v>40189</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12">
         <v>7352</v>
@@ -2449,16 +2449,16 @@
         <v>241</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12">
         <v>107</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H12" s="1">
         <v>40255</v>
@@ -2578,9 +2578,9 @@
         <v>40255</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13">
         <v>7466</v>
@@ -2589,16 +2589,16 @@
         <v>362</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13">
         <v>107</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H13" s="1">
         <v>40332</v>
@@ -2718,9 +2718,9 @@
         <v>40332</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>7372</v>
@@ -2729,16 +2729,16 @@
         <v>169</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14">
         <v>110</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H14" s="1">
         <v>40269</v>
@@ -2861,9 +2861,9 @@
         <v>41603</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <v>7620</v>
@@ -2872,16 +2872,16 @@
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15">
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="1">
         <v>40513</v>
@@ -3004,9 +3004,9 @@
         <v>40522</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16">
         <v>7618</v>
@@ -3015,16 +3015,16 @@
         <v>142</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16">
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H16" s="1">
         <v>40513</v>
@@ -3147,9 +3147,9 @@
         <v>40522</v>
       </c>
     </row>
-    <row r="17" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>7286</v>
@@ -3158,16 +3158,16 @@
         <v>141</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H17" s="1">
         <v>40234</v>
@@ -3248,7 +3248,7 @@
         <v>1</v>
       </c>
       <c r="AL17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM17">
         <v>-4</v>
@@ -3287,9 +3287,9 @@
         <v>40234</v>
       </c>
     </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18">
         <v>7344</v>
@@ -3298,16 +3298,16 @@
         <v>159</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18">
         <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H18" s="1">
         <v>40253</v>
@@ -3427,9 +3427,9 @@
         <v>40253</v>
       </c>
     </row>
-    <row r="19" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19">
         <v>7370</v>
@@ -3438,16 +3438,16 @@
         <v>276</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19">
         <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H19" s="1">
         <v>40268</v>
@@ -3567,9 +3567,9 @@
         <v>40268</v>
       </c>
     </row>
-    <row r="20" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>7424</v>
@@ -3578,16 +3578,16 @@
         <v>337</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20">
         <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H20" s="1">
         <v>40309</v>
@@ -3707,9 +3707,9 @@
         <v>40309</v>
       </c>
     </row>
-    <row r="21" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21">
         <v>7468</v>
@@ -3718,16 +3718,16 @@
         <v>424</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E21">
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" s="1">
         <v>40333</v>
@@ -3847,9 +3847,9 @@
         <v>40333</v>
       </c>
     </row>
-    <row r="22" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22">
         <v>7258</v>
@@ -3858,16 +3858,16 @@
         <v>96</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E22">
         <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H22" s="1">
         <v>40227</v>
@@ -3987,9 +3987,9 @@
         <v>40227</v>
       </c>
     </row>
-    <row r="23" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23">
         <v>7478</v>
@@ -3998,16 +3998,16 @@
         <v>130</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E23">
         <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H23" s="1">
         <v>40338</v>
@@ -4127,9 +4127,9 @@
         <v>40338</v>
       </c>
     </row>
-    <row r="24" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24">
         <v>6996</v>
@@ -4138,16 +4138,16 @@
         <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E24">
         <v>11</v>
       </c>
       <c r="F24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H24" s="1">
         <v>40109</v>
@@ -4267,9 +4267,9 @@
         <v>40109</v>
       </c>
     </row>
-    <row r="25" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25">
         <v>7356</v>
@@ -4278,16 +4278,16 @@
         <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E25">
         <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H25" s="1">
         <v>40255</v>
@@ -4407,9 +4407,9 @@
         <v>40255</v>
       </c>
     </row>
-    <row r="26" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26">
         <v>7358</v>
@@ -4418,16 +4418,16 @@
         <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E26">
         <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H26" s="1">
         <v>40259</v>
@@ -4547,9 +4547,9 @@
         <v>40259</v>
       </c>
     </row>
-    <row r="27" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27">
         <v>7306</v>
@@ -4558,16 +4558,16 @@
         <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E27">
         <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H27" s="1">
         <v>40238</v>
@@ -4687,9 +4687,9 @@
         <v>40238</v>
       </c>
     </row>
-    <row r="28" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28">
         <v>7350</v>
@@ -4698,16 +4698,16 @@
         <v>81</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E28">
         <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H28" s="1">
         <v>40255</v>
@@ -4827,9 +4827,9 @@
         <v>40255</v>
       </c>
     </row>
-    <row r="29" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29">
         <v>7322</v>
@@ -4838,16 +4838,16 @@
         <v>126</v>
       </c>
       <c r="D29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E29">
         <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H29" s="1">
         <v>40242</v>
@@ -4967,9 +4967,9 @@
         <v>40242</v>
       </c>
     </row>
-    <row r="30" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30">
         <v>7340</v>
@@ -4978,16 +4978,16 @@
         <v>217</v>
       </c>
       <c r="D30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E30">
         <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H30" s="1">
         <v>40249</v>
@@ -5107,9 +5107,9 @@
         <v>40249</v>
       </c>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31">
         <v>7416</v>
@@ -5118,16 +5118,16 @@
         <v>331</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E31">
         <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H31" s="1">
         <v>40304</v>
@@ -5247,9 +5247,9 @@
         <v>40304</v>
       </c>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32">
         <v>7376</v>
@@ -5258,16 +5258,16 @@
         <v>388</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E32">
         <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H32" s="1">
         <v>40270</v>
@@ -5387,9 +5387,9 @@
         <v>40270</v>
       </c>
     </row>
-    <row r="33" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33">
         <v>7156</v>
@@ -5398,16 +5398,16 @@
         <v>74</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E33">
         <v>13</v>
       </c>
       <c r="F33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H33" s="1">
         <v>40189</v>
@@ -5527,9 +5527,9 @@
         <v>40189</v>
       </c>
     </row>
-    <row r="34" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34">
         <v>7472</v>
@@ -5538,16 +5538,16 @@
         <v>116</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E34">
         <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H34" s="1">
         <v>40333</v>
@@ -5667,9 +5667,9 @@
         <v>40333</v>
       </c>
     </row>
-    <row r="35" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35">
         <v>7256</v>
@@ -5678,16 +5678,16 @@
         <v>118</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E35">
         <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H35" s="1">
         <v>40227</v>
@@ -5807,9 +5807,9 @@
         <v>40227</v>
       </c>
     </row>
-    <row r="36" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36">
         <v>7354</v>
@@ -5818,16 +5818,16 @@
         <v>120</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E36">
         <v>13</v>
       </c>
       <c r="F36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H36" s="1">
         <v>40255</v>
@@ -5947,9 +5947,9 @@
         <v>40255</v>
       </c>
     </row>
-    <row r="37" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37">
         <v>7476</v>
@@ -5958,16 +5958,16 @@
         <v>256</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E37">
         <v>13</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H37" s="1">
         <v>40338</v>
@@ -6087,9 +6087,9 @@
         <v>40338</v>
       </c>
     </row>
-    <row r="38" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38">
         <v>7464</v>
@@ -6098,16 +6098,16 @@
         <v>307</v>
       </c>
       <c r="D38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E38">
         <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H38" s="1">
         <v>40330</v>
@@ -6230,9 +6230,9 @@
         <v>40821</v>
       </c>
     </row>
-    <row r="39" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39">
         <v>7446</v>
@@ -6241,16 +6241,16 @@
         <v>403</v>
       </c>
       <c r="D39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E39">
         <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H39" s="1">
         <v>40322</v>
@@ -6370,9 +6370,9 @@
         <v>40322</v>
       </c>
     </row>
-    <row r="40" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40">
         <v>7444</v>
@@ -6381,16 +6381,16 @@
         <v>408</v>
       </c>
       <c r="D40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E40">
         <v>13</v>
       </c>
       <c r="F40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H40" s="1">
         <v>40322</v>
@@ -6513,9 +6513,9 @@
         <v>41544</v>
       </c>
     </row>
-    <row r="41" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41">
         <v>7496</v>
@@ -6524,16 +6524,16 @@
         <v>644</v>
       </c>
       <c r="D41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E41">
         <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H41" s="1">
         <v>40358</v>
@@ -6653,9 +6653,9 @@
         <v>40358</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B42">
         <v>7638</v>
@@ -6664,16 +6664,16 @@
         <v>835</v>
       </c>
       <c r="D42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E42">
         <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H42" s="1">
         <v>40539</v>
@@ -6793,9 +6793,9 @@
         <v>40539</v>
       </c>
     </row>
-    <row r="43" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43">
         <v>7518</v>
@@ -6804,16 +6804,16 @@
         <v>214</v>
       </c>
       <c r="D43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E43">
         <v>16</v>
       </c>
       <c r="F43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H43" s="1">
         <v>40387</v>
@@ -6933,9 +6933,9 @@
         <v>40387</v>
       </c>
     </row>
-    <row r="44" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>7520</v>
@@ -6944,16 +6944,16 @@
         <v>479</v>
       </c>
       <c r="D44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E44">
         <v>16</v>
       </c>
       <c r="F44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H44" s="1">
         <v>40387</v>
@@ -7073,9 +7073,9 @@
         <v>40387</v>
       </c>
     </row>
-    <row r="45" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45">
         <v>7534</v>
@@ -7084,16 +7084,16 @@
         <v>677</v>
       </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E45">
         <v>16</v>
       </c>
       <c r="F45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H45" s="1">
         <v>40401</v>
@@ -7213,9 +7213,9 @@
         <v>40401</v>
       </c>
     </row>
-    <row r="46" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46">
         <v>7486</v>
@@ -7224,16 +7224,16 @@
         <v>514</v>
       </c>
       <c r="D46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E46">
         <v>52</v>
       </c>
       <c r="F46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H46" s="1">
         <v>40345</v>
@@ -7317,7 +7317,7 @@
         <v>4.3750000000000004E-2</v>
       </c>
       <c r="AL46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AM46">
         <v>-4</v>
@@ -7356,9 +7356,9 @@
         <v>41774</v>
       </c>
     </row>
-    <row r="47" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47">
         <v>7526</v>
@@ -7367,16 +7367,16 @@
         <v>734</v>
       </c>
       <c r="D47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E47">
         <v>52</v>
       </c>
       <c r="F47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H47" s="1">
         <v>40399</v>
@@ -7496,9 +7496,9 @@
         <v>40399</v>
       </c>
     </row>
-    <row r="48" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48">
         <v>7528</v>
@@ -7507,16 +7507,16 @@
         <v>741</v>
       </c>
       <c r="D48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E48">
         <v>52</v>
       </c>
       <c r="F48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H48" s="1">
         <v>40399</v>
@@ -7636,9 +7636,9 @@
         <v>40399</v>
       </c>
     </row>
-    <row r="49" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49">
         <v>7316</v>
@@ -7647,16 +7647,16 @@
         <v>156</v>
       </c>
       <c r="D49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E49">
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H49" s="1">
         <v>40240</v>
@@ -7776,9 +7776,9 @@
         <v>40240</v>
       </c>
     </row>
-    <row r="50" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50">
         <v>7276</v>
@@ -7787,16 +7787,16 @@
         <v>204</v>
       </c>
       <c r="D50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E50">
         <v>6</v>
       </c>
       <c r="F50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H50" s="1">
         <v>40232</v>
@@ -7916,9 +7916,9 @@
         <v>40232</v>
       </c>
     </row>
-    <row r="51" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51">
         <v>7532</v>
@@ -7927,16 +7927,16 @@
         <v>303</v>
       </c>
       <c r="D51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E51">
         <v>18</v>
       </c>
       <c r="F51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H51" s="1">
         <v>40399</v>
@@ -8056,9 +8056,9 @@
         <v>40399</v>
       </c>
     </row>
-    <row r="52" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52">
         <v>7396</v>
@@ -8067,16 +8067,16 @@
         <v>467</v>
       </c>
       <c r="D52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E52">
         <v>18</v>
       </c>
       <c r="F52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H52" s="1">
         <v>40282</v>
@@ -8199,9 +8199,9 @@
         <v>40284</v>
       </c>
     </row>
-    <row r="53" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>7566</v>
@@ -8210,16 +8210,16 @@
         <v>539</v>
       </c>
       <c r="D53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E53">
         <v>18</v>
       </c>
       <c r="F53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H53" s="1">
         <v>40429</v>
@@ -8339,9 +8339,9 @@
         <v>40429</v>
       </c>
     </row>
-    <row r="54" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54">
         <v>7326</v>
@@ -8350,16 +8350,16 @@
         <v>125</v>
       </c>
       <c r="D54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E54">
         <v>20</v>
       </c>
       <c r="F54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H54" s="1">
         <v>40246</v>
@@ -8479,9 +8479,9 @@
         <v>40246</v>
       </c>
     </row>
-    <row r="55" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>7400</v>
@@ -8490,16 +8490,16 @@
         <v>262</v>
       </c>
       <c r="D55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E55">
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H55" s="1">
         <v>40284</v>
@@ -8619,9 +8619,9 @@
         <v>40284</v>
       </c>
     </row>
-    <row r="56" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56">
         <v>7470</v>
@@ -8630,16 +8630,16 @@
         <v>314</v>
       </c>
       <c r="D56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E56">
         <v>20</v>
       </c>
       <c r="F56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H56" s="1">
         <v>40333</v>
@@ -8762,9 +8762,9 @@
         <v>40333</v>
       </c>
     </row>
-    <row r="57" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57">
         <v>7644</v>
@@ -8773,16 +8773,16 @@
         <v>679</v>
       </c>
       <c r="D57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E57">
         <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H57" s="1">
         <v>40562</v>
@@ -8902,9 +8902,9 @@
         <v>40562</v>
       </c>
     </row>
-    <row r="58" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58">
         <v>7442</v>
@@ -8913,16 +8913,16 @@
         <v>389</v>
       </c>
       <c r="D58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E58">
         <v>58</v>
       </c>
       <c r="F58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H58" s="1">
         <v>40316</v>
@@ -9042,9 +9042,9 @@
         <v>40316</v>
       </c>
     </row>
-    <row r="59" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59">
         <v>7604</v>
@@ -9053,16 +9053,16 @@
         <v>919</v>
       </c>
       <c r="D59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E59">
         <v>58</v>
       </c>
       <c r="F59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H59" s="1">
         <v>40501</v>
@@ -9185,9 +9185,9 @@
         <v>40501</v>
       </c>
     </row>
-    <row r="60" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B60">
         <v>7422</v>
@@ -9196,16 +9196,16 @@
         <v>56</v>
       </c>
       <c r="D60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E60">
         <v>32</v>
       </c>
       <c r="F60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H60" s="1">
         <v>40308</v>
@@ -9325,9 +9325,9 @@
         <v>40308</v>
       </c>
     </row>
-    <row r="61" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B61">
         <v>7426</v>
@@ -9336,16 +9336,16 @@
         <v>59</v>
       </c>
       <c r="D61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E61">
         <v>32</v>
       </c>
       <c r="F61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H61" s="1">
         <v>40309</v>
@@ -9465,9 +9465,9 @@
         <v>40309</v>
       </c>
     </row>
-    <row r="62" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B62">
         <v>7522</v>
@@ -9476,16 +9476,16 @@
         <v>257</v>
       </c>
       <c r="D62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E62">
         <v>32</v>
       </c>
       <c r="F62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H62" s="1">
         <v>40396</v>
@@ -9605,9 +9605,9 @@
         <v>40396</v>
       </c>
     </row>
-    <row r="63" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B63">
         <v>7450</v>
@@ -9616,16 +9616,16 @@
         <v>127</v>
       </c>
       <c r="D63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E63">
         <v>33</v>
       </c>
       <c r="F63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H63" s="1">
         <v>40326</v>
@@ -9745,9 +9745,9 @@
         <v>40326</v>
       </c>
     </row>
-    <row r="64" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B64">
         <v>7452</v>
@@ -9756,16 +9756,16 @@
         <v>210</v>
       </c>
       <c r="D64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E64">
         <v>33</v>
       </c>
       <c r="F64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H64" s="1">
         <v>40326</v>
@@ -9885,9 +9885,9 @@
         <v>40326</v>
       </c>
     </row>
-    <row r="65" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B65">
         <v>7454</v>
@@ -9896,16 +9896,16 @@
         <v>401</v>
       </c>
       <c r="D65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E65">
         <v>33</v>
       </c>
       <c r="F65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H65" s="1">
         <v>40326</v>
@@ -10025,9 +10025,9 @@
         <v>40326</v>
       </c>
     </row>
-    <row r="66" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B66">
         <v>7456</v>
@@ -10036,16 +10036,16 @@
         <v>473</v>
       </c>
       <c r="D66" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E66">
         <v>33</v>
       </c>
       <c r="F66" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G66" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H66" s="1">
         <v>40326</v>
@@ -10165,9 +10165,9 @@
         <v>40326</v>
       </c>
     </row>
-    <row r="67" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B67">
         <v>7436</v>
@@ -10176,16 +10176,16 @@
         <v>315</v>
       </c>
       <c r="D67" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E67">
         <v>35</v>
       </c>
       <c r="F67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H67" s="1">
         <v>40313</v>
@@ -10305,9 +10305,9 @@
         <v>40313</v>
       </c>
     </row>
-    <row r="68" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B68">
         <v>7580</v>
@@ -10316,16 +10316,16 @@
         <v>311</v>
       </c>
       <c r="D68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E68">
         <v>36</v>
       </c>
       <c r="F68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H68" s="1">
         <v>40451</v>
@@ -10445,9 +10445,9 @@
         <v>40451</v>
       </c>
     </row>
-    <row r="69" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B69">
         <v>7514</v>
@@ -10456,16 +10456,16 @@
         <v>386</v>
       </c>
       <c r="D69" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E69">
         <v>36</v>
       </c>
       <c r="F69" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G69" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H69" s="1">
         <v>40381</v>
@@ -10585,9 +10585,9 @@
         <v>40381</v>
       </c>
     </row>
-    <row r="70" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B70">
         <v>7266</v>
@@ -10596,16 +10596,16 @@
         <v>160</v>
       </c>
       <c r="D70" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E70">
         <v>44</v>
       </c>
       <c r="F70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H70" s="1">
         <v>40228</v>
@@ -10725,9 +10725,9 @@
         <v>40228</v>
       </c>
     </row>
-    <row r="71" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B71">
         <v>7328</v>
@@ -10736,16 +10736,16 @@
         <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E71">
         <v>44</v>
       </c>
       <c r="F71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H71" s="1">
         <v>40246</v>
@@ -10865,9 +10865,9 @@
         <v>40246</v>
       </c>
     </row>
-    <row r="72" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B72">
         <v>7386</v>
@@ -10876,16 +10876,16 @@
         <v>172</v>
       </c>
       <c r="D72" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E72">
         <v>44</v>
       </c>
       <c r="F72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H72" s="1">
         <v>40275</v>
@@ -11005,9 +11005,9 @@
         <v>40275</v>
       </c>
     </row>
-    <row r="73" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B73">
         <v>7392</v>
@@ -11016,16 +11016,16 @@
         <v>269</v>
       </c>
       <c r="D73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E73">
         <v>44</v>
       </c>
       <c r="F73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H73" s="1">
         <v>40281</v>
@@ -11145,9 +11145,9 @@
         <v>40281</v>
       </c>
     </row>
-    <row r="74" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B74">
         <v>7410</v>
@@ -11156,16 +11156,16 @@
         <v>352</v>
       </c>
       <c r="D74" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E74">
         <v>45</v>
       </c>
       <c r="F74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H74" s="1">
         <v>40298</v>
@@ -11285,9 +11285,9 @@
         <v>40298</v>
       </c>
     </row>
-    <row r="75" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B75">
         <v>7440</v>
@@ -11296,16 +11296,16 @@
         <v>361</v>
       </c>
       <c r="D75" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E75">
         <v>5</v>
       </c>
       <c r="F75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H75" s="1">
         <v>40316</v>
@@ -11425,9 +11425,9 @@
         <v>40316</v>
       </c>
     </row>
-    <row r="76" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B76">
         <v>7538</v>
@@ -11436,16 +11436,16 @@
         <v>382</v>
       </c>
       <c r="D76" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E76">
         <v>5</v>
       </c>
       <c r="F76" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G76" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H76" s="1">
         <v>40402</v>
@@ -11565,9 +11565,9 @@
         <v>40402</v>
       </c>
     </row>
-    <row r="77" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B77">
         <v>7548</v>
@@ -11576,16 +11576,16 @@
         <v>752</v>
       </c>
       <c r="D77" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E77">
         <v>5</v>
       </c>
       <c r="F77" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G77" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H77" s="1">
         <v>40416</v>
@@ -11705,9 +11705,9 @@
         <v>40416</v>
       </c>
     </row>
-    <row r="78" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B78">
         <v>7634</v>
@@ -11716,16 +11716,16 @@
         <v>72</v>
       </c>
       <c r="D78" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E78">
         <v>94</v>
       </c>
       <c r="F78" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G78" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H78" s="1">
         <v>40520</v>
@@ -11845,9 +11845,9 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="79" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B79">
         <v>7632</v>
@@ -11856,16 +11856,16 @@
         <v>106</v>
       </c>
       <c r="D79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E79">
         <v>94</v>
       </c>
       <c r="F79" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G79" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H79" s="1">
         <v>40520</v>
@@ -11985,9 +11985,9 @@
         <v>40520</v>
       </c>
     </row>
-    <row r="80" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B80">
         <v>7630</v>
@@ -11996,16 +11996,16 @@
         <v>108</v>
       </c>
       <c r="D80" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E80">
         <v>94</v>
       </c>
       <c r="F80" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G80" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H80" s="1">
         <v>40519</v>
@@ -12125,9 +12125,9 @@
         <v>40519</v>
       </c>
     </row>
-    <row r="81" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B81">
         <v>7628</v>
@@ -12136,16 +12136,16 @@
         <v>113</v>
       </c>
       <c r="D81" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E81">
         <v>94</v>
       </c>
       <c r="F81" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G81" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H81" s="1">
         <v>40519</v>
@@ -12265,9 +12265,9 @@
         <v>40519</v>
       </c>
     </row>
-    <row r="82" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B82">
         <v>7626</v>
@@ -12276,16 +12276,16 @@
         <v>298</v>
       </c>
       <c r="D82" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E82">
         <v>94</v>
       </c>
       <c r="F82" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G82" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H82" s="1">
         <v>40519</v>
@@ -12405,9 +12405,9 @@
         <v>40519</v>
       </c>
     </row>
-    <row r="83" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B83">
         <v>7494</v>
@@ -12416,16 +12416,16 @@
         <v>605</v>
       </c>
       <c r="D83" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E83">
         <v>113</v>
       </c>
       <c r="F83" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G83" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H83" s="1">
         <v>40358</v>
@@ -12545,9 +12545,9 @@
         <v>40358</v>
       </c>
     </row>
-    <row r="84" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B84">
         <v>7510</v>
@@ -12556,16 +12556,16 @@
         <v>680</v>
       </c>
       <c r="D84" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E84">
         <v>113</v>
       </c>
       <c r="F84" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G84" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H84" s="1">
         <v>40379</v>
@@ -12685,9 +12685,9 @@
         <v>40379</v>
       </c>
     </row>
-    <row r="85" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B85">
         <v>7506</v>
@@ -12696,16 +12696,16 @@
         <v>708</v>
       </c>
       <c r="D85" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E85">
         <v>113</v>
       </c>
       <c r="F85" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G85" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H85" s="1">
         <v>40371</v>
@@ -12825,9 +12825,9 @@
         <v>40371</v>
       </c>
     </row>
-    <row r="86" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B86">
         <v>7536</v>
@@ -12836,16 +12836,16 @@
         <v>709</v>
       </c>
       <c r="D86" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E86">
         <v>113</v>
       </c>
       <c r="F86" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G86" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H86" s="1">
         <v>40401</v>
@@ -12965,9 +12965,9 @@
         <v>40401</v>
       </c>
     </row>
-    <row r="87" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B87">
         <v>7636</v>
@@ -12976,16 +12976,16 @@
         <v>1077</v>
       </c>
       <c r="D87" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E87">
         <v>113</v>
       </c>
       <c r="F87" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G87" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H87" s="1">
         <v>40532</v>
@@ -13108,9 +13108,9 @@
         <v>40651</v>
       </c>
     </row>
-    <row r="88" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B88">
         <v>7212</v>
@@ -13119,16 +13119,16 @@
         <v>112</v>
       </c>
       <c r="D88" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E88">
         <v>114</v>
       </c>
       <c r="F88" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G88" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H88" s="1">
         <v>40218</v>
@@ -13248,9 +13248,9 @@
         <v>40218</v>
       </c>
     </row>
-    <row r="89" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B89">
         <v>7398</v>
@@ -13259,16 +13259,16 @@
         <v>259</v>
       </c>
       <c r="D89" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E89">
         <v>114</v>
       </c>
       <c r="F89" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G89" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H89" s="1">
         <v>40283</v>
@@ -13388,9 +13388,9 @@
         <v>40283</v>
       </c>
     </row>
-    <row r="90" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B90">
         <v>7430</v>
@@ -13399,16 +13399,16 @@
         <v>260</v>
       </c>
       <c r="D90" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E90">
         <v>114</v>
       </c>
       <c r="F90" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G90" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H90" s="1">
         <v>40310</v>
@@ -13528,9 +13528,9 @@
         <v>40310</v>
       </c>
     </row>
-    <row r="91" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B91">
         <v>7730</v>
@@ -13539,16 +13539,16 @@
         <v>232</v>
       </c>
       <c r="D91" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E91">
         <v>117</v>
       </c>
       <c r="F91" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G91" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H91" s="1">
         <v>41829</v>
@@ -13668,9 +13668,9 @@
         <v>41829</v>
       </c>
     </row>
-    <row r="92" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B92">
         <v>7606</v>
@@ -13679,16 +13679,16 @@
         <v>285</v>
       </c>
       <c r="D92" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E92">
         <v>117</v>
       </c>
       <c r="F92" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G92" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H92" s="1">
         <v>40511</v>
@@ -13808,9 +13808,9 @@
         <v>40511</v>
       </c>
     </row>
-    <row r="93" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B93">
         <v>7734</v>
@@ -13819,16 +13819,16 @@
         <v>289</v>
       </c>
       <c r="D93" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E93">
         <v>117</v>
       </c>
       <c r="F93" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G93" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H93" s="1">
         <v>41830</v>
@@ -13948,9 +13948,9 @@
         <v>41830</v>
       </c>
     </row>
-    <row r="94" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B94">
         <v>7608</v>
@@ -13959,16 +13959,16 @@
         <v>505</v>
       </c>
       <c r="D94" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E94">
         <v>117</v>
       </c>
       <c r="F94" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G94" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H94" s="1">
         <v>40511</v>
@@ -14088,9 +14088,9 @@
         <v>40511</v>
       </c>
     </row>
-    <row r="95" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B95">
         <v>7614</v>
@@ -14099,16 +14099,16 @@
         <v>886</v>
       </c>
       <c r="D95" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E95">
         <v>117</v>
       </c>
       <c r="F95" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G95" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H95" s="1">
         <v>40513</v>
@@ -14228,9 +14228,9 @@
         <v>40513</v>
       </c>
     </row>
-    <row r="96" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B96">
         <v>7610</v>
@@ -14239,16 +14239,16 @@
         <v>969</v>
       </c>
       <c r="D96" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E96">
         <v>117</v>
       </c>
       <c r="F96" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G96" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H96" s="1">
         <v>40511</v>
@@ -14368,9 +14368,9 @@
         <v>40511</v>
       </c>
     </row>
-    <row r="97" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B97">
         <v>7204</v>
@@ -14379,16 +14379,16 @@
         <v>123</v>
       </c>
       <c r="D97" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E97">
         <v>118</v>
       </c>
       <c r="F97" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G97" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H97" s="1">
         <v>40213</v>
@@ -14508,9 +14508,9 @@
         <v>40213</v>
       </c>
     </row>
-    <row r="98" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B98">
         <v>7502</v>
@@ -14519,16 +14519,16 @@
         <v>384</v>
       </c>
       <c r="D98" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E98">
         <v>118</v>
       </c>
       <c r="F98" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G98" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H98" s="1">
         <v>40359</v>
@@ -14648,9 +14648,9 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="99" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B99">
         <v>7428</v>
@@ -14659,16 +14659,16 @@
         <v>441</v>
       </c>
       <c r="D99" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E99">
         <v>118</v>
       </c>
       <c r="F99" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G99" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H99" s="1">
         <v>40310</v>
@@ -14791,9 +14791,9 @@
         <v>40310</v>
       </c>
     </row>
-    <row r="100" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B100">
         <v>7500</v>
@@ -14802,16 +14802,16 @@
         <v>86</v>
       </c>
       <c r="D100" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E100">
         <v>123</v>
       </c>
       <c r="F100" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G100" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H100" s="1">
         <v>40359</v>
@@ -14931,9 +14931,9 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="101" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B101">
         <v>7498</v>
@@ -14942,16 +14942,16 @@
         <v>107</v>
       </c>
       <c r="D101" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E101">
         <v>123</v>
       </c>
       <c r="F101" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G101" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H101" s="1">
         <v>40359</v>
@@ -15071,9 +15071,9 @@
         <v>40359</v>
       </c>
     </row>
-    <row r="102" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B102">
         <v>7448</v>
@@ -15082,16 +15082,16 @@
         <v>186</v>
       </c>
       <c r="D102" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E102">
         <v>123</v>
       </c>
       <c r="F102" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G102" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H102" s="1">
         <v>40323</v>

</xml_diff>